<commit_message>
some updates for NWES MP1.07
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-07-04.xlsx
+++ b/EC/Train Runs and Enforcements 2016-07-04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Train Runs" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="686">
   <si>
     <t>Train ID</t>
   </si>
@@ -2117,9 +2117,6 @@
   </si>
   <si>
     <t>No issue found… any insights from ops?</t>
-  </si>
-  <si>
-    <t>Mismatched CRC between subdiv and WIU</t>
   </si>
 </sst>
 </file>
@@ -2780,7 +2777,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_XINGS" xfId="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -3183,7 +3187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -21468,37 +21472,37 @@
     <mergeCell ref="I3:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="W11:W12 W13:X1048576">
-    <cfRule type="cellIs" dxfId="11" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="75" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X1048576">
-    <cfRule type="cellIs" dxfId="10" priority="58" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="58" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:X1048576">
-    <cfRule type="cellIs" dxfId="9" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:S14 A13:J13 L13:S13 A15:J139 A141:J156 K15:S209">
-    <cfRule type="expression" dxfId="8" priority="51">
+    <cfRule type="expression" dxfId="9" priority="51">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:S14 A13:J13 L13:S13 A15:J139 A141:J156 K15:S209">
-    <cfRule type="expression" dxfId="7" priority="50">
+    <cfRule type="expression" dxfId="8" priority="50">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>$O13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>$P13&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21543,8 +21547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N55" sqref="A55:N55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70:N75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25058,7 +25062,7 @@
         <v>121</v>
       </c>
       <c r="N71" s="11" t="s">
-        <v>686</v>
+        <v>159</v>
       </c>
       <c r="O71" s="1"/>
       <c r="P71" s="43" t="str">
@@ -25112,7 +25116,7 @@
         <v>121</v>
       </c>
       <c r="N72" s="11" t="s">
-        <v>686</v>
+        <v>159</v>
       </c>
       <c r="O72" s="1"/>
       <c r="P72" s="43" t="str">
@@ -25166,7 +25170,7 @@
         <v>121</v>
       </c>
       <c r="N73" s="11" t="s">
-        <v>686</v>
+        <v>159</v>
       </c>
       <c r="O73" s="1"/>
       <c r="P73" s="43" t="str">
@@ -25220,7 +25224,7 @@
         <v>121</v>
       </c>
       <c r="N74" s="11" t="s">
-        <v>686</v>
+        <v>159</v>
       </c>
       <c r="P74" s="43" t="str">
         <f>VLOOKUP(C74,'Train Runs'!$A$13:$V$972,22,0)</f>
@@ -25273,7 +25277,7 @@
         <v>121</v>
       </c>
       <c r="N75" s="11" t="s">
-        <v>686</v>
+        <v>159</v>
       </c>
       <c r="P75" s="43" t="str">
         <f>VLOOKUP(C75,'Train Runs'!$A$13:$V$972,22,0)</f>
@@ -28025,17 +28029,17 @@
     <mergeCell ref="A5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="P6 M6:N6 M7:M1048576">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:N7 A8:K75 L8:N128">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>$M7="Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M3">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>